<commit_message>
update hach toan cuoi ky
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/data/xml/template_lsx_v2.xlsx
+++ b/addons/custom/forlife_purchase/data/xml/template_lsx_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FW\odoo\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\data\xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A102413-ED22-4D4F-A90F-4894BDA550BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE28130-2E18-4FB8-BEF9-862FA07B7FA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sản phẩm hoàn thành" sheetId="1" r:id="rId1"/>
@@ -163,9 +163,6 @@
     <t>642_CPC</t>
   </si>
   <si>
-    <t>Mã thành phẩm</t>
-  </si>
-  <si>
     <t>Size M</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>Phân loại sản xuất</t>
+  </si>
+  <si>
+    <t>Mã sản phẩm</t>
   </si>
 </sst>
 </file>
@@ -739,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>4</v>
@@ -782,16 +782,16 @@
         <v>5</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>41</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>42</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>6</v>
@@ -853,10 +853,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
         <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
       </c>
       <c r="C5" s="2">
         <v>1111000000</v>
@@ -910,7 +910,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -930,16 +930,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>38</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>12</v>
@@ -975,7 +975,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
@@ -1002,7 +1002,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
@@ -1048,7 +1048,7 @@
     </row>
     <row r="5" spans="1:11" ht="27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>22</v>
@@ -1058,7 +1058,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
@@ -1085,7 +1085,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
@@ -1139,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B37E9D6-9C3B-444F-A145-F09B13187BCA}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1155,7 +1155,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>25</v>
@@ -1170,7 +1170,7 @@
         <v>28</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1208,7 +1208,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>30</v>

</xml_diff>